<commit_message>
Added wishme , made data.csv usable for mow but the index is still not functionable
</commit_message>
<xml_diff>
--- a/Features/Features.xlsx
+++ b/Features/Features.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\AI----Project\AI---Project\Features\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\CODING PLAYGROUND\CODE\Jarvis AI\Features\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A589B98-0409-4280-BF0A-AD2D828B7157}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D77B3013-00F5-4EEB-8957-229459CB72F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -404,17 +404,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="17.28515625" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -425,7 +425,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -436,7 +436,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -447,7 +447,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -458,7 +458,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -469,7 +469,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -480,7 +480,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -491,7 +491,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
@@ -502,7 +502,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -513,7 +513,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
@@ -524,7 +524,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
@@ -535,7 +535,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
@@ -546,7 +546,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
@@ -557,7 +557,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13</v>
       </c>
@@ -568,7 +568,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>14</v>
       </c>
@@ -579,7 +579,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>15</v>
       </c>
@@ -590,7 +590,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>16</v>
       </c>

</xml_diff>

<commit_message>
Added the wait feature, removed some bugs and added features description in the features,xlsx file
</commit_message>
<xml_diff>
--- a/Features/Features.xlsx
+++ b/Features/Features.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\CODING PLAYGROUND\CODE\Jarvis AI\Features\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D77B3013-00F5-4EEB-8957-229459CB72F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F59EB49-1E16-4416-9FA3-C0EEE5111187}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="44">
   <si>
     <t>Index</t>
   </si>
@@ -85,6 +85,78 @@
   </si>
   <si>
     <t>CSV Writer</t>
+  </si>
+  <si>
+    <t>Repeat</t>
+  </si>
+  <si>
+    <t>Function</t>
+  </si>
+  <si>
+    <t>speaks</t>
+  </si>
+  <si>
+    <t>listens</t>
+  </si>
+  <si>
+    <t>wishes w.r.t current time</t>
+  </si>
+  <si>
+    <t>Tells the top 5 news</t>
+  </si>
+  <si>
+    <t>Tells a programming joke</t>
+  </si>
+  <si>
+    <t>Sets an alarm</t>
+  </si>
+  <si>
+    <t>States the current loaction w.r.t. IP address</t>
+  </si>
+  <si>
+    <t>It has 2 modes first tells only temp and weather type and second says wind speed and humidity</t>
+  </si>
+  <si>
+    <t>Current date</t>
+  </si>
+  <si>
+    <t>Current time</t>
+  </si>
+  <si>
+    <t>Today's day</t>
+  </si>
+  <si>
+    <t>reads the first five lines from the wikipedia</t>
+  </si>
+  <si>
+    <t>searches a particular item on google</t>
+  </si>
+  <si>
+    <t xml:space="preserve">used for any random search </t>
+  </si>
+  <si>
+    <t>opens photos on google</t>
+  </si>
+  <si>
+    <t>writes all the responses and queries with date and time on the data.csv file</t>
+  </si>
+  <si>
+    <t>Reads the last respons from the data.csv</t>
+  </si>
+  <si>
+    <t>Wolframssl</t>
+  </si>
+  <si>
+    <t>wolfram</t>
+  </si>
+  <si>
+    <t>If it doesn’t understand anything it searches it on the wolphram api , but then we need an Id here</t>
+  </si>
+  <si>
+    <t>wait function</t>
+  </si>
+  <si>
+    <t xml:space="preserve">it waits for first 10 secs and then if asked to wait more it waits for the given time; </t>
   </si>
 </sst>
 </file>
@@ -402,19 +474,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:C18"/>
+  <dimension ref="A2:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="17.33203125" customWidth="1"/>
     <col min="3" max="3" width="18.33203125" customWidth="1"/>
+    <col min="4" max="4" width="93.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -424,8 +497,11 @@
       <c r="C2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -435,8 +511,11 @@
       <c r="C3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -446,8 +525,11 @@
       <c r="C4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -457,8 +539,11 @@
       <c r="C5" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -468,8 +553,11 @@
       <c r="C6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -479,8 +567,11 @@
       <c r="C7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -490,8 +581,11 @@
       <c r="C8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
@@ -501,8 +595,11 @@
       <c r="C9" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -512,8 +609,11 @@
       <c r="C10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
@@ -523,8 +623,11 @@
       <c r="C11" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
@@ -534,8 +637,11 @@
       <c r="C12" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
@@ -545,8 +651,11 @@
       <c r="C13" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
@@ -556,8 +665,11 @@
       <c r="C14" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13</v>
       </c>
@@ -567,8 +679,11 @@
       <c r="C15" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>14</v>
       </c>
@@ -578,8 +693,11 @@
       <c r="C16" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>15</v>
       </c>
@@ -589,8 +707,11 @@
       <c r="C17" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>16</v>
       </c>
@@ -599,6 +720,51 @@
       </c>
       <c r="C18" t="s">
         <v>19</v>
+      </c>
+      <c r="D18" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" t="s">
+        <v>40</v>
+      </c>
+      <c r="D20" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>